<commit_message>
Pequeño fix en la hoja de cálculo.
</commit_message>
<xml_diff>
--- a/AHP.xlsx
+++ b/AHP.xlsx
@@ -255,7 +255,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -264,9 +264,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -277,6 +274,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="3" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -285,9 +285,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -760,8 +757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM986"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R40" sqref="R40:R43"/>
+    <sheetView tabSelected="1" topLeftCell="F25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J56" sqref="J56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -844,7 +841,7 @@
       <c r="V2" s="2"/>
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
-      <c r="Y2" s="9"/>
+      <c r="Y2" s="8"/>
       <c r="Z2"/>
       <c r="AA2"/>
       <c r="AB2"/>
@@ -924,7 +921,7 @@
       <c r="X3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="Y3" s="9"/>
+      <c r="Y3" s="8"/>
       <c r="Z3"/>
       <c r="AA3"/>
       <c r="AB3"/>
@@ -945,66 +942,66 @@
       <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="6">
-        <v>1</v>
-      </c>
-      <c r="D4" s="6">
-        <v>1</v>
-      </c>
-      <c r="E4" s="6">
-        <v>1</v>
-      </c>
-      <c r="F4" s="6">
+      <c r="C4" s="5">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5">
         <v>1</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="6">
-        <v>1</v>
-      </c>
-      <c r="J4" s="6">
-        <v>1</v>
-      </c>
-      <c r="K4" s="6">
-        <v>1</v>
-      </c>
-      <c r="L4" s="6">
+      <c r="I4" s="5">
+        <v>1</v>
+      </c>
+      <c r="J4" s="5">
+        <v>1</v>
+      </c>
+      <c r="K4" s="5">
+        <v>1</v>
+      </c>
+      <c r="L4" s="5">
         <v>1</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="6">
-        <v>1</v>
-      </c>
-      <c r="P4" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="6">
-        <v>1</v>
-      </c>
-      <c r="R4" s="6">
+      <c r="O4" s="5">
+        <v>1</v>
+      </c>
+      <c r="P4" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>1</v>
+      </c>
+      <c r="R4" s="5">
         <v>1</v>
       </c>
       <c r="T4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="U4" s="6">
-        <v>1</v>
-      </c>
-      <c r="V4" s="6">
-        <v>1</v>
-      </c>
-      <c r="W4" s="6">
-        <v>1</v>
-      </c>
-      <c r="X4" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y4" s="9"/>
+      <c r="U4" s="5">
+        <v>1</v>
+      </c>
+      <c r="V4" s="5">
+        <v>1</v>
+      </c>
+      <c r="W4" s="5">
+        <v>1</v>
+      </c>
+      <c r="X4" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="8"/>
       <c r="Z4"/>
       <c r="AA4"/>
       <c r="AB4"/>
@@ -1025,70 +1022,70 @@
       <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <f>1/D4</f>
         <v>1</v>
       </c>
-      <c r="D5" s="6">
-        <v>1</v>
-      </c>
-      <c r="E5" s="6">
-        <v>1</v>
-      </c>
-      <c r="F5" s="6">
+      <c r="D5" s="5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5">
         <v>1</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="5">
         <f>1/J4</f>
         <v>1</v>
       </c>
-      <c r="J5" s="6">
-        <v>1</v>
-      </c>
-      <c r="K5" s="6">
-        <v>1</v>
-      </c>
-      <c r="L5" s="6">
+      <c r="J5" s="5">
+        <v>1</v>
+      </c>
+      <c r="K5" s="5">
+        <v>1</v>
+      </c>
+      <c r="L5" s="5">
         <v>1</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="O5" s="6">
+      <c r="O5" s="5">
         <f>1/P4</f>
         <v>1</v>
       </c>
-      <c r="P5" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="6">
-        <v>1</v>
-      </c>
-      <c r="R5" s="6">
+      <c r="P5" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>1</v>
+      </c>
+      <c r="R5" s="5">
         <v>1</v>
       </c>
       <c r="T5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="U5" s="6">
+      <c r="U5" s="5">
         <f>1/V4</f>
         <v>1</v>
       </c>
-      <c r="V5" s="6">
-        <v>1</v>
-      </c>
-      <c r="W5" s="6">
-        <v>1</v>
-      </c>
-      <c r="X5" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y5" s="9"/>
+      <c r="V5" s="5">
+        <v>1</v>
+      </c>
+      <c r="W5" s="5">
+        <v>1</v>
+      </c>
+      <c r="X5" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="8"/>
       <c r="Z5"/>
       <c r="AA5"/>
       <c r="AB5"/>
@@ -1109,74 +1106,74 @@
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <f>1/E4</f>
         <v>1</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <f>1/E5</f>
         <v>1</v>
       </c>
-      <c r="E6" s="6">
-        <v>1</v>
-      </c>
-      <c r="F6" s="6">
+      <c r="E6" s="5">
+        <v>1</v>
+      </c>
+      <c r="F6" s="5">
         <v>1</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="5">
         <f>1/K4</f>
         <v>1</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="5">
         <f>1/K5</f>
         <v>1</v>
       </c>
-      <c r="K6" s="6">
-        <v>1</v>
-      </c>
-      <c r="L6" s="6">
+      <c r="K6" s="5">
+        <v>1</v>
+      </c>
+      <c r="L6" s="5">
         <v>1</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="O6" s="6">
+      <c r="O6" s="5">
         <f>1/Q4</f>
         <v>1</v>
       </c>
-      <c r="P6" s="6">
+      <c r="P6" s="5">
         <f>1/Q5</f>
         <v>1</v>
       </c>
-      <c r="Q6" s="6">
-        <v>1</v>
-      </c>
-      <c r="R6" s="6">
+      <c r="Q6" s="5">
+        <v>1</v>
+      </c>
+      <c r="R6" s="5">
         <v>1</v>
       </c>
       <c r="T6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="U6" s="6">
+      <c r="U6" s="5">
         <f>1/W4</f>
         <v>1</v>
       </c>
-      <c r="V6" s="6">
+      <c r="V6" s="5">
         <f>1/W5</f>
         <v>1</v>
       </c>
-      <c r="W6" s="6">
-        <v>1</v>
-      </c>
-      <c r="X6" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y6" s="9"/>
+      <c r="W6" s="5">
+        <v>1</v>
+      </c>
+      <c r="X6" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="8"/>
       <c r="Z6"/>
       <c r="AA6"/>
       <c r="AB6"/>
@@ -1197,78 +1194,78 @@
       <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <f>1/F4</f>
         <v>1</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <f>1/F5</f>
         <v>1</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <f>1/F6</f>
         <v>1</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>1</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="5">
         <f>1/L4</f>
         <v>1</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="5">
         <f>1/L5</f>
         <v>1</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K7" s="5">
         <f>1/L6</f>
         <v>1</v>
       </c>
-      <c r="L7" s="6">
+      <c r="L7" s="5">
         <v>1</v>
       </c>
       <c r="M7" s="2"/>
       <c r="N7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O7" s="6">
+      <c r="O7" s="5">
         <f>1/R4</f>
         <v>1</v>
       </c>
-      <c r="P7" s="6">
+      <c r="P7" s="5">
         <f>1/R5</f>
         <v>1</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="Q7" s="5">
         <f>1/R6</f>
         <v>1</v>
       </c>
-      <c r="R7" s="6">
+      <c r="R7" s="5">
         <v>1</v>
       </c>
       <c r="T7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="U7" s="6">
+      <c r="U7" s="5">
         <f>1/X4</f>
         <v>1</v>
       </c>
-      <c r="V7" s="6">
+      <c r="V7" s="5">
         <f>1/X5</f>
         <v>1</v>
       </c>
-      <c r="W7" s="6">
+      <c r="W7" s="5">
         <f>1/X6</f>
         <v>1</v>
       </c>
-      <c r="X7" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y7" s="9"/>
+      <c r="X7" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="8"/>
       <c r="Z7"/>
       <c r="AA7"/>
       <c r="AB7"/>
@@ -1308,7 +1305,7 @@
       <c r="V8" s="2"/>
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
-      <c r="Y8" s="9"/>
+      <c r="Y8" s="8"/>
       <c r="Z8"/>
       <c r="AA8"/>
       <c r="AB8"/>
@@ -1356,7 +1353,7 @@
       <c r="V9" s="2"/>
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
-      <c r="Y9" s="9"/>
+      <c r="Y9" s="8"/>
       <c r="Z9"/>
       <c r="AA9"/>
       <c r="AB9"/>
@@ -1436,7 +1433,7 @@
       <c r="X10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Y10" s="9"/>
+      <c r="Y10" s="8"/>
       <c r="Z10"/>
       <c r="AA10"/>
       <c r="AB10"/>
@@ -1457,66 +1454,66 @@
       <c r="B11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="6">
-        <v>1</v>
-      </c>
-      <c r="D11" s="6">
+      <c r="C11" s="5">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5">
         <v>0.125</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>0.1</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="5">
         <v>0.125</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="6">
-        <v>1</v>
-      </c>
-      <c r="J11" s="6">
+      <c r="I11" s="5">
+        <v>1</v>
+      </c>
+      <c r="J11" s="5">
         <v>0.7142857142857143</v>
       </c>
-      <c r="K11" s="6">
+      <c r="K11" s="5">
         <v>0.83333333333333337</v>
       </c>
-      <c r="L11" s="6">
+      <c r="L11" s="5">
         <v>0.5</v>
       </c>
       <c r="M11" s="2"/>
       <c r="N11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="O11" s="6">
-        <v>1</v>
-      </c>
-      <c r="P11" s="6">
+      <c r="O11" s="5">
+        <v>1</v>
+      </c>
+      <c r="P11" s="5">
         <v>1.2857142857142858</v>
       </c>
-      <c r="Q11" s="6">
+      <c r="Q11" s="5">
         <v>4.5</v>
       </c>
-      <c r="R11" s="6">
+      <c r="R11" s="5">
         <v>9</v>
       </c>
       <c r="T11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="U11" s="6">
-        <v>1</v>
-      </c>
-      <c r="V11" s="6">
+      <c r="U11" s="5">
+        <v>1</v>
+      </c>
+      <c r="V11" s="5">
         <v>5</v>
       </c>
-      <c r="W11" s="6">
+      <c r="W11" s="5">
         <v>1.6666666666666667</v>
       </c>
-      <c r="X11" s="6">
+      <c r="X11" s="5">
         <v>1.4285714285714286</v>
       </c>
-      <c r="Y11" s="9"/>
+      <c r="Y11" s="8"/>
       <c r="Z11"/>
       <c r="AA11"/>
       <c r="AB11"/>
@@ -1537,66 +1534,66 @@
       <c r="B12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>8</v>
       </c>
-      <c r="D12" s="6">
-        <v>1</v>
-      </c>
-      <c r="E12" s="6">
+      <c r="D12" s="5">
+        <v>1</v>
+      </c>
+      <c r="E12" s="5">
         <v>0.8</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="5">
         <v>1</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="5">
         <v>1.4</v>
       </c>
-      <c r="J12" s="6">
-        <v>1</v>
-      </c>
-      <c r="K12" s="6">
+      <c r="J12" s="5">
+        <v>1</v>
+      </c>
+      <c r="K12" s="5">
         <v>1.1666666666666667</v>
       </c>
-      <c r="L12" s="6">
+      <c r="L12" s="5">
         <v>0.7</v>
       </c>
       <c r="M12" s="2"/>
       <c r="N12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="O12" s="6">
+      <c r="O12" s="5">
         <v>0.77777777777777768</v>
       </c>
-      <c r="P12" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="6">
+      <c r="P12" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="5">
         <v>3.4999999999999996</v>
       </c>
-      <c r="R12" s="6">
+      <c r="R12" s="5">
         <v>6.9999999999999991</v>
       </c>
       <c r="T12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="U12" s="6">
+      <c r="U12" s="5">
         <v>0.2</v>
       </c>
-      <c r="V12" s="6">
-        <v>1</v>
-      </c>
-      <c r="W12" s="6">
+      <c r="V12" s="5">
+        <v>1</v>
+      </c>
+      <c r="W12" s="5">
         <v>0.33333333333333337</v>
       </c>
-      <c r="X12" s="6">
+      <c r="X12" s="5">
         <v>0.28571428571428575</v>
       </c>
-      <c r="Y12" s="9"/>
+      <c r="Y12" s="8"/>
       <c r="Z12"/>
       <c r="AA12"/>
       <c r="AB12"/>
@@ -1617,66 +1614,66 @@
       <c r="B13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>10</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <v>1.25</v>
       </c>
-      <c r="E13" s="6">
-        <v>1</v>
-      </c>
-      <c r="F13" s="6">
+      <c r="E13" s="5">
+        <v>1</v>
+      </c>
+      <c r="F13" s="5">
         <v>1.25</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13" s="5">
         <v>1.2</v>
       </c>
-      <c r="J13" s="6">
+      <c r="J13" s="5">
         <v>0.8571428571428571</v>
       </c>
-      <c r="K13" s="6">
-        <v>1</v>
-      </c>
-      <c r="L13" s="6">
+      <c r="K13" s="5">
+        <v>1</v>
+      </c>
+      <c r="L13" s="5">
         <v>0.6</v>
       </c>
       <c r="M13" s="2"/>
       <c r="N13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O13" s="6">
+      <c r="O13" s="5">
         <v>0.22222222222222221</v>
       </c>
-      <c r="P13" s="6">
+      <c r="P13" s="5">
         <v>0.28571428571428575</v>
       </c>
-      <c r="Q13" s="6">
-        <v>1</v>
-      </c>
-      <c r="R13" s="6">
+      <c r="Q13" s="5">
+        <v>1</v>
+      </c>
+      <c r="R13" s="5">
         <v>2</v>
       </c>
       <c r="T13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="U13" s="6">
+      <c r="U13" s="5">
         <v>0.6</v>
       </c>
-      <c r="V13" s="6">
+      <c r="V13" s="5">
         <v>2.9999999999999996</v>
       </c>
-      <c r="W13" s="6">
-        <v>1</v>
-      </c>
-      <c r="X13" s="6">
+      <c r="W13" s="5">
+        <v>1</v>
+      </c>
+      <c r="X13" s="5">
         <v>0.85714285714285721</v>
       </c>
-      <c r="Y13" s="9"/>
+      <c r="Y13" s="8"/>
       <c r="Z13"/>
       <c r="AA13"/>
       <c r="AB13"/>
@@ -1697,66 +1694,66 @@
       <c r="B14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <v>8</v>
       </c>
-      <c r="D14" s="6">
-        <v>1</v>
-      </c>
-      <c r="E14" s="6">
+      <c r="D14" s="5">
+        <v>1</v>
+      </c>
+      <c r="E14" s="5">
         <v>0.8</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="5">
         <v>1</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="6">
+      <c r="I14" s="5">
         <v>2</v>
       </c>
-      <c r="J14" s="6">
+      <c r="J14" s="5">
         <v>1.4285714285714286</v>
       </c>
-      <c r="K14" s="6">
+      <c r="K14" s="5">
         <v>1.6666666666666667</v>
       </c>
-      <c r="L14" s="6">
+      <c r="L14" s="5">
         <v>1</v>
       </c>
       <c r="M14" s="2"/>
       <c r="N14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O14" s="6">
+      <c r="O14" s="5">
         <v>0.1111111111111111</v>
       </c>
-      <c r="P14" s="6">
+      <c r="P14" s="5">
         <v>0.14285714285714288</v>
       </c>
-      <c r="Q14" s="6">
+      <c r="Q14" s="5">
         <v>0.5</v>
       </c>
-      <c r="R14" s="6">
+      <c r="R14" s="5">
         <v>1</v>
       </c>
       <c r="T14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U14" s="6">
+      <c r="U14" s="5">
         <v>0.7</v>
       </c>
-      <c r="V14" s="6">
+      <c r="V14" s="5">
         <v>3.4999999999999996</v>
       </c>
-      <c r="W14" s="6">
+      <c r="W14" s="5">
         <v>1.1666666666666665</v>
       </c>
-      <c r="X14" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y14" s="9"/>
+      <c r="X14" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y14" s="8"/>
       <c r="Z14"/>
       <c r="AA14"/>
       <c r="AB14"/>
@@ -1796,7 +1793,7 @@
       <c r="V15" s="2"/>
       <c r="W15" s="2"/>
       <c r="X15" s="2"/>
-      <c r="Y15" s="9"/>
+      <c r="Y15" s="8"/>
       <c r="Z15"/>
       <c r="AA15"/>
       <c r="AB15"/>
@@ -1844,7 +1841,7 @@
       <c r="V16" s="2"/>
       <c r="W16" s="2"/>
       <c r="X16" s="2"/>
-      <c r="Y16" s="9"/>
+      <c r="Y16" s="8"/>
       <c r="Z16"/>
       <c r="AA16"/>
       <c r="AB16"/>
@@ -1924,7 +1921,7 @@
       <c r="X17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Y17" s="9"/>
+      <c r="Y17" s="8"/>
       <c r="Z17"/>
       <c r="AA17"/>
       <c r="AB17"/>
@@ -1945,66 +1942,66 @@
       <c r="B18" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="6">
-        <v>1</v>
-      </c>
-      <c r="D18" s="6">
+      <c r="C18" s="5">
+        <v>1</v>
+      </c>
+      <c r="D18" s="5">
         <v>3</v>
       </c>
-      <c r="E18" s="6">
-        <v>1</v>
-      </c>
-      <c r="F18" s="6">
+      <c r="E18" s="5">
+        <v>1</v>
+      </c>
+      <c r="F18" s="5">
         <v>1.5</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I18" s="6">
-        <v>1</v>
-      </c>
-      <c r="J18" s="6">
+      <c r="I18" s="5">
+        <v>1</v>
+      </c>
+      <c r="J18" s="5">
         <v>1.5</v>
       </c>
-      <c r="K18" s="6">
+      <c r="K18" s="5">
         <v>1.5</v>
       </c>
-      <c r="L18" s="6">
+      <c r="L18" s="5">
         <v>1.5</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="O18" s="6">
-        <v>1</v>
-      </c>
-      <c r="P18" s="6">
+      <c r="O18" s="5">
+        <v>1</v>
+      </c>
+      <c r="P18" s="5">
         <v>0.66666666666666663</v>
       </c>
-      <c r="Q18" s="6">
-        <v>1</v>
-      </c>
-      <c r="R18" s="6">
+      <c r="Q18" s="5">
+        <v>1</v>
+      </c>
+      <c r="R18" s="5">
         <v>1</v>
       </c>
       <c r="T18" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="U18" s="6">
-        <v>1</v>
-      </c>
-      <c r="V18" s="6">
+      <c r="U18" s="5">
+        <v>1</v>
+      </c>
+      <c r="V18" s="5">
         <v>3</v>
       </c>
-      <c r="W18" s="6">
-        <v>1</v>
-      </c>
-      <c r="X18" s="6">
+      <c r="W18" s="5">
+        <v>1</v>
+      </c>
+      <c r="X18" s="5">
         <v>1.5</v>
       </c>
-      <c r="Y18" s="9"/>
+      <c r="Y18" s="8"/>
       <c r="Z18"/>
       <c r="AA18"/>
       <c r="AB18"/>
@@ -2025,66 +2022,66 @@
       <c r="B19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="5">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D19" s="6">
-        <v>1</v>
-      </c>
-      <c r="E19" s="6">
+      <c r="D19" s="5">
+        <v>1</v>
+      </c>
+      <c r="E19" s="5">
         <v>0.33333333333333331</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="5">
         <v>0.5</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I19" s="6">
+      <c r="I19" s="5">
         <v>0.66666666666666663</v>
       </c>
-      <c r="J19" s="6">
-        <v>1</v>
-      </c>
-      <c r="K19" s="6">
-        <v>1</v>
-      </c>
-      <c r="L19" s="6">
+      <c r="J19" s="5">
+        <v>1</v>
+      </c>
+      <c r="K19" s="5">
+        <v>1</v>
+      </c>
+      <c r="L19" s="5">
         <v>1</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="O19" s="6">
+      <c r="O19" s="5">
         <v>1.5</v>
       </c>
-      <c r="P19" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q19" s="6">
+      <c r="P19" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="5">
         <v>1.5</v>
       </c>
-      <c r="R19" s="6">
+      <c r="R19" s="5">
         <v>1.5</v>
       </c>
       <c r="T19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="U19" s="6">
+      <c r="U19" s="5">
         <v>0.33333333333333331</v>
       </c>
-      <c r="V19" s="6">
-        <v>1</v>
-      </c>
-      <c r="W19" s="6">
+      <c r="V19" s="5">
+        <v>1</v>
+      </c>
+      <c r="W19" s="5">
         <v>0.33333333333333331</v>
       </c>
-      <c r="X19" s="6">
+      <c r="X19" s="5">
         <v>0.5</v>
       </c>
-      <c r="Y19" s="9"/>
+      <c r="Y19" s="8"/>
       <c r="Z19"/>
       <c r="AA19"/>
       <c r="AB19"/>
@@ -2105,66 +2102,66 @@
       <c r="B20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="6">
-        <v>1</v>
-      </c>
-      <c r="D20" s="6">
+      <c r="C20" s="5">
+        <v>1</v>
+      </c>
+      <c r="D20" s="5">
         <v>3</v>
       </c>
-      <c r="E20" s="6">
-        <v>1</v>
-      </c>
-      <c r="F20" s="6">
+      <c r="E20" s="5">
+        <v>1</v>
+      </c>
+      <c r="F20" s="5">
         <v>1.5</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I20" s="6">
+      <c r="I20" s="5">
         <v>0.66666666666666663</v>
       </c>
-      <c r="J20" s="6">
-        <v>1</v>
-      </c>
-      <c r="K20" s="6">
-        <v>1</v>
-      </c>
-      <c r="L20" s="6">
+      <c r="J20" s="5">
+        <v>1</v>
+      </c>
+      <c r="K20" s="5">
+        <v>1</v>
+      </c>
+      <c r="L20" s="5">
         <v>1</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O20" s="6">
-        <v>1</v>
-      </c>
-      <c r="P20" s="6">
+      <c r="O20" s="5">
+        <v>1</v>
+      </c>
+      <c r="P20" s="5">
         <v>0.66666666666666663</v>
       </c>
-      <c r="Q20" s="6">
-        <v>1</v>
-      </c>
-      <c r="R20" s="6">
+      <c r="Q20" s="5">
+        <v>1</v>
+      </c>
+      <c r="R20" s="5">
         <v>1</v>
       </c>
       <c r="T20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="U20" s="6">
-        <v>1</v>
-      </c>
-      <c r="V20" s="6">
+      <c r="U20" s="5">
+        <v>1</v>
+      </c>
+      <c r="V20" s="5">
         <v>3</v>
       </c>
-      <c r="W20" s="6">
-        <v>1</v>
-      </c>
-      <c r="X20" s="6">
+      <c r="W20" s="5">
+        <v>1</v>
+      </c>
+      <c r="X20" s="5">
         <v>1.5</v>
       </c>
-      <c r="Y20" s="9"/>
+      <c r="Y20" s="8"/>
       <c r="Z20"/>
       <c r="AA20"/>
       <c r="AB20"/>
@@ -2185,66 +2182,66 @@
       <c r="B21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="5">
         <v>0.66666666666666663</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="5">
         <v>2</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="5">
         <v>0.66666666666666663</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="5">
         <v>1</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I21" s="6">
+      <c r="I21" s="5">
         <v>0.66666666666666663</v>
       </c>
-      <c r="J21" s="6">
-        <v>1</v>
-      </c>
-      <c r="K21" s="6">
-        <v>1</v>
-      </c>
-      <c r="L21" s="6">
+      <c r="J21" s="5">
+        <v>1</v>
+      </c>
+      <c r="K21" s="5">
+        <v>1</v>
+      </c>
+      <c r="L21" s="5">
         <v>1</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O21" s="6">
-        <v>1</v>
-      </c>
-      <c r="P21" s="6">
+      <c r="O21" s="5">
+        <v>1</v>
+      </c>
+      <c r="P21" s="5">
         <v>0.66666666666666663</v>
       </c>
-      <c r="Q21" s="6">
-        <v>1</v>
-      </c>
-      <c r="R21" s="6">
+      <c r="Q21" s="5">
+        <v>1</v>
+      </c>
+      <c r="R21" s="5">
         <v>1</v>
       </c>
       <c r="T21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U21" s="6">
+      <c r="U21" s="5">
         <v>0.66666666666666663</v>
       </c>
-      <c r="V21" s="6">
+      <c r="V21" s="5">
         <v>2</v>
       </c>
-      <c r="W21" s="6">
+      <c r="W21" s="5">
         <v>0.66666666666666663</v>
       </c>
-      <c r="X21" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y21" s="9"/>
+      <c r="X21" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y21" s="8"/>
       <c r="Z21"/>
       <c r="AA21"/>
       <c r="AB21"/>
@@ -2284,7 +2281,7 @@
       <c r="V22" s="2"/>
       <c r="W22" s="2"/>
       <c r="X22" s="2"/>
-      <c r="Y22" s="9"/>
+      <c r="Y22" s="8"/>
       <c r="Z22"/>
       <c r="AA22"/>
       <c r="AB22"/>
@@ -2332,7 +2329,7 @@
       <c r="V23" s="2"/>
       <c r="W23" s="2"/>
       <c r="X23" s="2"/>
-      <c r="Y23" s="9"/>
+      <c r="Y23" s="8"/>
       <c r="Z23"/>
       <c r="AA23"/>
       <c r="AB23"/>
@@ -2412,7 +2409,7 @@
       <c r="X24" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Y24" s="9"/>
+      <c r="Y24" s="8"/>
       <c r="Z24"/>
       <c r="AA24"/>
       <c r="AB24"/>
@@ -2433,66 +2430,66 @@
       <c r="B25" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="6">
-        <v>1</v>
-      </c>
-      <c r="D25" s="6">
+      <c r="C25" s="5">
+        <v>1</v>
+      </c>
+      <c r="D25" s="5">
         <v>0.5</v>
       </c>
-      <c r="E25" s="6">
-        <v>1</v>
-      </c>
-      <c r="F25" s="6">
+      <c r="E25" s="5">
+        <v>1</v>
+      </c>
+      <c r="F25" s="5">
         <v>0.5</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I25" s="6">
-        <v>1</v>
-      </c>
-      <c r="J25" s="6">
-        <v>1</v>
-      </c>
-      <c r="K25" s="6">
-        <v>1</v>
-      </c>
-      <c r="L25" s="6">
+      <c r="I25" s="5">
+        <v>1</v>
+      </c>
+      <c r="J25" s="5">
+        <v>1</v>
+      </c>
+      <c r="K25" s="5">
+        <v>1</v>
+      </c>
+      <c r="L25" s="5">
         <v>1</v>
       </c>
       <c r="M25" s="2"/>
       <c r="N25" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="O25" s="6">
-        <v>1</v>
-      </c>
-      <c r="P25" s="6">
+      <c r="O25" s="5">
+        <v>1</v>
+      </c>
+      <c r="P25" s="5">
         <v>0.5</v>
       </c>
-      <c r="Q25" s="6">
+      <c r="Q25" s="5">
         <v>0.5</v>
       </c>
-      <c r="R25" s="6">
+      <c r="R25" s="5">
         <v>1</v>
       </c>
       <c r="T25" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="U25" s="6">
-        <v>1</v>
-      </c>
-      <c r="V25" s="6">
-        <v>1</v>
-      </c>
-      <c r="W25" s="6">
-        <v>1</v>
-      </c>
-      <c r="X25" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y25" s="9"/>
+      <c r="U25" s="5">
+        <v>1</v>
+      </c>
+      <c r="V25" s="5">
+        <v>1</v>
+      </c>
+      <c r="W25" s="5">
+        <v>1</v>
+      </c>
+      <c r="X25" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y25" s="8"/>
       <c r="Z25"/>
       <c r="AA25"/>
       <c r="AB25"/>
@@ -2513,66 +2510,66 @@
       <c r="B26" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="5">
         <v>2</v>
       </c>
-      <c r="D26" s="6">
-        <v>1</v>
-      </c>
-      <c r="E26" s="6">
+      <c r="D26" s="5">
+        <v>1</v>
+      </c>
+      <c r="E26" s="5">
         <v>2</v>
       </c>
-      <c r="F26" s="6">
+      <c r="F26" s="5">
         <v>1</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I26" s="6">
-        <v>1</v>
-      </c>
-      <c r="J26" s="6">
-        <v>1</v>
-      </c>
-      <c r="K26" s="6">
-        <v>1</v>
-      </c>
-      <c r="L26" s="6">
+      <c r="I26" s="5">
+        <v>1</v>
+      </c>
+      <c r="J26" s="5">
+        <v>1</v>
+      </c>
+      <c r="K26" s="5">
+        <v>1</v>
+      </c>
+      <c r="L26" s="5">
         <v>1</v>
       </c>
       <c r="M26" s="2"/>
       <c r="N26" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="O26" s="6">
+      <c r="O26" s="5">
         <v>2</v>
       </c>
-      <c r="P26" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q26" s="6">
-        <v>1</v>
-      </c>
-      <c r="R26" s="6">
+      <c r="P26" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="5">
+        <v>1</v>
+      </c>
+      <c r="R26" s="5">
         <v>2</v>
       </c>
       <c r="T26" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="U26" s="6">
-        <v>1</v>
-      </c>
-      <c r="V26" s="6">
-        <v>1</v>
-      </c>
-      <c r="W26" s="6">
-        <v>1</v>
-      </c>
-      <c r="X26" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y26" s="9"/>
+      <c r="U26" s="5">
+        <v>1</v>
+      </c>
+      <c r="V26" s="5">
+        <v>1</v>
+      </c>
+      <c r="W26" s="5">
+        <v>1</v>
+      </c>
+      <c r="X26" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y26" s="8"/>
       <c r="Z26"/>
       <c r="AA26"/>
       <c r="AB26"/>
@@ -2593,66 +2590,66 @@
       <c r="B27" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="6">
-        <v>1</v>
-      </c>
-      <c r="D27" s="6">
+      <c r="C27" s="5">
+        <v>1</v>
+      </c>
+      <c r="D27" s="5">
         <v>0.5</v>
       </c>
-      <c r="E27" s="6">
-        <v>1</v>
-      </c>
-      <c r="F27" s="6">
+      <c r="E27" s="5">
+        <v>1</v>
+      </c>
+      <c r="F27" s="5">
         <v>0.5</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I27" s="6">
-        <v>1</v>
-      </c>
-      <c r="J27" s="6">
-        <v>1</v>
-      </c>
-      <c r="K27" s="6">
-        <v>1</v>
-      </c>
-      <c r="L27" s="6">
+      <c r="I27" s="5">
+        <v>1</v>
+      </c>
+      <c r="J27" s="5">
+        <v>1</v>
+      </c>
+      <c r="K27" s="5">
+        <v>1</v>
+      </c>
+      <c r="L27" s="5">
         <v>1</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O27" s="6">
+      <c r="O27" s="5">
         <v>2</v>
       </c>
-      <c r="P27" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q27" s="6">
-        <v>1</v>
-      </c>
-      <c r="R27" s="6">
+      <c r="P27" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="5">
+        <v>1</v>
+      </c>
+      <c r="R27" s="5">
         <v>2</v>
       </c>
       <c r="T27" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="U27" s="6">
-        <v>1</v>
-      </c>
-      <c r="V27" s="6">
-        <v>1</v>
-      </c>
-      <c r="W27" s="6">
-        <v>1</v>
-      </c>
-      <c r="X27" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y27" s="9"/>
+      <c r="U27" s="5">
+        <v>1</v>
+      </c>
+      <c r="V27" s="5">
+        <v>1</v>
+      </c>
+      <c r="W27" s="5">
+        <v>1</v>
+      </c>
+      <c r="X27" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y27" s="8"/>
       <c r="Z27"/>
       <c r="AA27"/>
       <c r="AB27"/>
@@ -2673,66 +2670,66 @@
       <c r="B28" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="5">
         <v>2</v>
       </c>
-      <c r="D28" s="6">
-        <v>1</v>
-      </c>
-      <c r="E28" s="6">
+      <c r="D28" s="5">
+        <v>1</v>
+      </c>
+      <c r="E28" s="5">
         <v>2</v>
       </c>
-      <c r="F28" s="6">
+      <c r="F28" s="5">
         <v>1</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I28" s="6">
-        <v>1</v>
-      </c>
-      <c r="J28" s="6">
-        <v>1</v>
-      </c>
-      <c r="K28" s="6">
-        <v>1</v>
-      </c>
-      <c r="L28" s="6">
+      <c r="I28" s="5">
+        <v>1</v>
+      </c>
+      <c r="J28" s="5">
+        <v>1</v>
+      </c>
+      <c r="K28" s="5">
+        <v>1</v>
+      </c>
+      <c r="L28" s="5">
         <v>1</v>
       </c>
       <c r="M28" s="2"/>
       <c r="N28" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O28" s="6">
-        <v>1</v>
-      </c>
-      <c r="P28" s="6">
+      <c r="O28" s="5">
+        <v>1</v>
+      </c>
+      <c r="P28" s="5">
         <v>0.5</v>
       </c>
-      <c r="Q28" s="6">
+      <c r="Q28" s="5">
         <v>0.5</v>
       </c>
-      <c r="R28" s="6">
+      <c r="R28" s="5">
         <v>1</v>
       </c>
       <c r="T28" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U28" s="6">
-        <v>1</v>
-      </c>
-      <c r="V28" s="6">
-        <v>1</v>
-      </c>
-      <c r="W28" s="6">
-        <v>1</v>
-      </c>
-      <c r="X28" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y28" s="9"/>
+      <c r="U28" s="5">
+        <v>1</v>
+      </c>
+      <c r="V28" s="5">
+        <v>1</v>
+      </c>
+      <c r="W28" s="5">
+        <v>1</v>
+      </c>
+      <c r="X28" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y28" s="8"/>
       <c r="Z28"/>
       <c r="AA28"/>
       <c r="AB28"/>
@@ -2772,7 +2769,7 @@
       <c r="V29" s="2"/>
       <c r="W29" s="2"/>
       <c r="X29" s="2"/>
-      <c r="Y29" s="9"/>
+      <c r="Y29" s="8"/>
       <c r="Z29"/>
       <c r="AA29"/>
       <c r="AB29"/>
@@ -2820,7 +2817,7 @@
       <c r="V30" s="2"/>
       <c r="W30" s="2"/>
       <c r="X30" s="2"/>
-      <c r="Y30" s="9"/>
+      <c r="Y30" s="8"/>
       <c r="Z30"/>
       <c r="AA30"/>
       <c r="AB30"/>
@@ -2900,7 +2897,7 @@
       <c r="X31" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Y31" s="9"/>
+      <c r="Y31" s="8"/>
       <c r="Z31"/>
       <c r="AA31"/>
       <c r="AB31"/>
@@ -2921,66 +2918,66 @@
       <c r="B32" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C32" s="6">
-        <v>1</v>
-      </c>
-      <c r="D32" s="6">
-        <v>1</v>
-      </c>
-      <c r="E32" s="6">
+      <c r="C32" s="5">
+        <v>1</v>
+      </c>
+      <c r="D32" s="5">
+        <v>1</v>
+      </c>
+      <c r="E32" s="5">
         <v>0.5</v>
       </c>
-      <c r="F32" s="6">
+      <c r="F32" s="5">
         <v>1</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I32" s="6">
-        <v>1</v>
-      </c>
-      <c r="J32" s="6">
+      <c r="I32" s="5">
+        <v>1</v>
+      </c>
+      <c r="J32" s="5">
         <v>0.33333333333333331</v>
       </c>
-      <c r="K32" s="6">
+      <c r="K32" s="5">
         <v>0.33333333333333331</v>
       </c>
-      <c r="L32" s="6">
+      <c r="L32" s="5">
         <v>0.5</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="O32" s="6">
-        <v>1</v>
-      </c>
-      <c r="P32" s="6">
+      <c r="O32" s="5">
+        <v>1</v>
+      </c>
+      <c r="P32" s="5">
         <v>2</v>
       </c>
-      <c r="Q32" s="6">
+      <c r="Q32" s="5">
         <v>0.66666666666666663</v>
       </c>
-      <c r="R32" s="6">
+      <c r="R32" s="5">
         <v>1</v>
       </c>
       <c r="T32" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="U32" s="6">
-        <v>1</v>
-      </c>
-      <c r="V32" s="6">
+      <c r="U32" s="5">
+        <v>1</v>
+      </c>
+      <c r="V32" s="5">
         <v>0.33333333333333331</v>
       </c>
-      <c r="W32" s="6">
-        <v>1</v>
-      </c>
-      <c r="X32" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y32" s="9"/>
+      <c r="W32" s="5">
+        <v>1</v>
+      </c>
+      <c r="X32" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y32" s="8"/>
       <c r="Z32"/>
       <c r="AA32"/>
       <c r="AB32"/>
@@ -3001,66 +2998,66 @@
       <c r="B33" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="6">
-        <v>1</v>
-      </c>
-      <c r="D33" s="6">
-        <v>1</v>
-      </c>
-      <c r="E33" s="6">
+      <c r="C33" s="5">
+        <v>1</v>
+      </c>
+      <c r="D33" s="5">
+        <v>1</v>
+      </c>
+      <c r="E33" s="5">
         <v>0.5</v>
       </c>
-      <c r="F33" s="6">
+      <c r="F33" s="5">
         <v>1</v>
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I33" s="6">
+      <c r="I33" s="5">
         <v>3</v>
       </c>
-      <c r="J33" s="6">
-        <v>1</v>
-      </c>
-      <c r="K33" s="6">
-        <v>1</v>
-      </c>
-      <c r="L33" s="6">
+      <c r="J33" s="5">
+        <v>1</v>
+      </c>
+      <c r="K33" s="5">
+        <v>1</v>
+      </c>
+      <c r="L33" s="5">
         <v>1.5</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="O33" s="6">
+      <c r="O33" s="5">
         <v>0.5</v>
       </c>
-      <c r="P33" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q33" s="6">
+      <c r="P33" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="5">
         <v>0.33333333333333331</v>
       </c>
-      <c r="R33" s="6">
+      <c r="R33" s="5">
         <v>0.5</v>
       </c>
       <c r="T33" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="U33" s="6">
+      <c r="U33" s="5">
         <v>3</v>
       </c>
-      <c r="V33" s="6">
-        <v>1</v>
-      </c>
-      <c r="W33" s="6">
+      <c r="V33" s="5">
+        <v>1</v>
+      </c>
+      <c r="W33" s="5">
         <v>3</v>
       </c>
-      <c r="X33" s="6">
+      <c r="X33" s="5">
         <v>3</v>
       </c>
-      <c r="Y33" s="9"/>
+      <c r="Y33" s="8"/>
       <c r="Z33"/>
       <c r="AA33"/>
       <c r="AB33"/>
@@ -3081,66 +3078,66 @@
       <c r="B34" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C34" s="5">
         <v>2</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D34" s="5">
         <v>2</v>
       </c>
-      <c r="E34" s="6">
-        <v>1</v>
-      </c>
-      <c r="F34" s="6">
+      <c r="E34" s="5">
+        <v>1</v>
+      </c>
+      <c r="F34" s="5">
         <v>2</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I34" s="6">
+      <c r="I34" s="5">
         <v>3</v>
       </c>
-      <c r="J34" s="6">
-        <v>1</v>
-      </c>
-      <c r="K34" s="6">
-        <v>1</v>
-      </c>
-      <c r="L34" s="6">
+      <c r="J34" s="5">
+        <v>1</v>
+      </c>
+      <c r="K34" s="5">
+        <v>1</v>
+      </c>
+      <c r="L34" s="5">
         <v>1.5</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O34" s="6">
+      <c r="O34" s="5">
         <v>1.5</v>
       </c>
-      <c r="P34" s="6">
+      <c r="P34" s="5">
         <v>3</v>
       </c>
-      <c r="Q34" s="6">
-        <v>1</v>
-      </c>
-      <c r="R34" s="6">
+      <c r="Q34" s="5">
+        <v>1</v>
+      </c>
+      <c r="R34" s="5">
         <v>1.5</v>
       </c>
       <c r="T34" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="U34" s="6">
-        <v>1</v>
-      </c>
-      <c r="V34" s="6">
+      <c r="U34" s="5">
+        <v>1</v>
+      </c>
+      <c r="V34" s="5">
         <v>0.33333333333333331</v>
       </c>
-      <c r="W34" s="6">
-        <v>1</v>
-      </c>
-      <c r="X34" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y34" s="9"/>
+      <c r="W34" s="5">
+        <v>1</v>
+      </c>
+      <c r="X34" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y34" s="8"/>
       <c r="Z34"/>
       <c r="AA34"/>
       <c r="AB34"/>
@@ -3161,66 +3158,66 @@
       <c r="B35" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C35" s="6">
-        <v>1</v>
-      </c>
-      <c r="D35" s="6">
-        <v>1</v>
-      </c>
-      <c r="E35" s="6">
+      <c r="C35" s="5">
+        <v>1</v>
+      </c>
+      <c r="D35" s="5">
+        <v>1</v>
+      </c>
+      <c r="E35" s="5">
         <v>0.5</v>
       </c>
-      <c r="F35" s="6">
+      <c r="F35" s="5">
         <v>1</v>
       </c>
       <c r="G35" s="2"/>
       <c r="H35" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I35" s="6">
+      <c r="I35" s="5">
         <v>2</v>
       </c>
-      <c r="J35" s="6">
+      <c r="J35" s="5">
         <v>0.66666666666666663</v>
       </c>
-      <c r="K35" s="6">
+      <c r="K35" s="5">
         <v>0.66666666666666663</v>
       </c>
-      <c r="L35" s="6">
+      <c r="L35" s="5">
         <v>1</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O35" s="6">
-        <v>1</v>
-      </c>
-      <c r="P35" s="6">
+      <c r="O35" s="5">
+        <v>1</v>
+      </c>
+      <c r="P35" s="5">
         <v>2</v>
       </c>
-      <c r="Q35" s="6">
+      <c r="Q35" s="5">
         <v>0.66666666666666663</v>
       </c>
-      <c r="R35" s="6">
+      <c r="R35" s="5">
         <v>1</v>
       </c>
       <c r="T35" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U35" s="6">
-        <v>1</v>
-      </c>
-      <c r="V35" s="6">
+      <c r="U35" s="5">
+        <v>1</v>
+      </c>
+      <c r="V35" s="5">
         <v>0.33333333333333331</v>
       </c>
-      <c r="W35" s="6">
-        <v>1</v>
-      </c>
-      <c r="X35" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y35" s="9"/>
+      <c r="W35" s="5">
+        <v>1</v>
+      </c>
+      <c r="X35" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y35" s="8"/>
       <c r="Z35"/>
       <c r="AA35"/>
       <c r="AB35"/>
@@ -3255,7 +3252,7 @@
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
       <c r="R36" s="2"/>
-      <c r="Y36" s="10"/>
+      <c r="Y36" s="9"/>
       <c r="Z36"/>
       <c r="AA36"/>
       <c r="AB36"/>
@@ -3266,30 +3263,30 @@
     </row>
     <row r="37" spans="1:39" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
-      <c r="I37" s="7"/>
-      <c r="J37" s="7"/>
-      <c r="K37" s="7"/>
-      <c r="L37" s="7"/>
-      <c r="M37" s="7"/>
-      <c r="N37" s="7"/>
-      <c r="O37" s="7"/>
-      <c r="P37" s="7"/>
-      <c r="Q37" s="7"/>
-      <c r="R37" s="7"/>
-      <c r="S37" s="7"/>
-      <c r="T37" s="7"/>
-      <c r="U37" s="7"/>
-      <c r="V37" s="7"/>
-      <c r="W37" s="7"/>
-      <c r="X37" s="7"/>
-      <c r="Y37" s="7"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+      <c r="N37" s="6"/>
+      <c r="O37" s="6"/>
+      <c r="P37" s="6"/>
+      <c r="Q37" s="6"/>
+      <c r="R37" s="6"/>
+      <c r="S37" s="6"/>
+      <c r="T37" s="6"/>
+      <c r="U37" s="6"/>
+      <c r="V37" s="6"/>
+      <c r="W37" s="6"/>
+      <c r="X37" s="6"/>
+      <c r="Y37" s="6"/>
       <c r="Z37"/>
       <c r="AA37"/>
       <c r="AB37"/>
@@ -3312,12 +3309,12 @@
       </c>
       <c r="I38" s="11"/>
       <c r="K38" s="11" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="L38" s="11"/>
       <c r="M38"/>
       <c r="N38" s="11" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="O38" s="11"/>
       <c r="Q38" s="11" t="s">
@@ -3358,17 +3355,17 @@
         <v>8</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="L39" s="4" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="M39"/>
       <c r="N39" s="3" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="O39" s="4" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="Q39" s="3" t="s">
         <v>6</v>
@@ -3395,45 +3392,45 @@
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="D40" s="6">
-        <f>(D4^$O$40*J4^$O$41*P4^$O$42*V4^$O$43)^(1/4)</f>
-        <v>1</v>
-      </c>
-      <c r="E40" s="6">
-        <f>(E4^$O$40*K4^$O$41*Q4^$O$42*W4^$O$43)^(1/4)</f>
-        <v>1</v>
-      </c>
-      <c r="F40" s="6">
-        <f>(F4^$O$40*L4^$O$41*R4^$O$42*X4^$O$43)^(1/4)</f>
+      <c r="D40" s="5">
+        <f>(D4^$L$40*J4^$L$41*P4^$L$42*V4^$L$43)^(1/4)</f>
+        <v>1</v>
+      </c>
+      <c r="E40" s="5">
+        <f>(E4^$L$40*K4^$L$41*Q4^$L$42*W4^$L$43)^(1/4)</f>
+        <v>1</v>
+      </c>
+      <c r="F40" s="5">
+        <f>(F4^$L$40*L4^$L$41*R4^$L$42*X4^$L$43)^(1/4)</f>
         <v>1</v>
       </c>
       <c r="H40" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I40" s="6">
+      <c r="I40" s="5">
         <f>(C40*D40*E40*F40)^(1/4)</f>
         <v>1</v>
       </c>
       <c r="K40" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L40" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="M40"/>
+      <c r="N40" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L40" s="8">
+      <c r="O40" s="7">
         <f>I40/SUM(I$40:I$43)</f>
         <v>0.25</v>
       </c>
-      <c r="M40"/>
-      <c r="N40" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="O40" s="8">
-        <v>0.25</v>
-      </c>
       <c r="Q40" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R40" s="14">
-        <f>L$40*O47+L$41*P47+L$42*Q47+L$43*R47</f>
-        <v>0.32615884159180875</v>
+      <c r="R40" s="10">
+        <f>O$40*O47+O$41*P47+O$42*Q47+O$43*R47</f>
+        <v>0.24564023900922094</v>
       </c>
       <c r="S40" s="2"/>
       <c r="Y40" s="2"/>
@@ -3450,7 +3447,7 @@
       <c r="B41" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C41" s="6">
+      <c r="C41" s="5">
         <f>1/D40</f>
         <v>1</v>
       </c>
@@ -3458,41 +3455,41 @@
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="E41" s="6">
-        <f>(E5^$O$40*K5^$O$41*Q5^$O$42*W5^$O$43)^(1/4)</f>
-        <v>1</v>
-      </c>
-      <c r="F41" s="6">
-        <f>(F5^$O$40*L5^$O$41*R5^$O$42*X5^$O$43)^(1/4)</f>
+      <c r="E41" s="5">
+        <f>(E5^$L$40*K5^$L$41*Q5^$L$42*W5^$L$43)^(1/4)</f>
+        <v>1</v>
+      </c>
+      <c r="F41" s="5">
+        <f>(F5^$L$40*L5^$L$41*R5^$L$42*X5^$L$43)^(1/4)</f>
         <v>1</v>
       </c>
       <c r="H41" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I41" s="6">
+      <c r="I41" s="5">
         <f>(C41*D41*E41*F41)^(1/4)</f>
         <v>1</v>
       </c>
       <c r="K41" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L41" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="M41"/>
+      <c r="N41" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L41" s="8">
+      <c r="O41" s="7">
         <f>I41/SUM(I$40:I$43)</f>
         <v>0.25</v>
       </c>
-      <c r="M41"/>
-      <c r="N41" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="O41" s="8">
-        <v>0.25</v>
-      </c>
       <c r="Q41" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="R41" s="14">
-        <f>L$40*O48+L$41*P48+L$42*Q48+L$43*R48</f>
-        <v>0.33257953816293695</v>
+      <c r="R41" s="10">
+        <f>O$40*O48+O$41*P48+O$42*Q48+O$43*R48</f>
+        <v>0.25046129707403497</v>
       </c>
       <c r="S41" s="2"/>
       <c r="Y41" s="2"/>
@@ -3509,7 +3506,7 @@
       <c r="B42" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C42" s="6">
+      <c r="C42" s="5">
         <f>1/E40</f>
         <v>1</v>
       </c>
@@ -3521,37 +3518,37 @@
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="F42" s="6">
-        <f>(F6^$O$40*L6^$O$41*R6^$O$42*X6^$O$43)^(1/4)</f>
+      <c r="F42" s="5">
+        <f>(F6^$L$40*L6^$L$41*R6^$L$42*X6^$L$43)^(1/4)</f>
         <v>1</v>
       </c>
       <c r="H42" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I42" s="6">
+      <c r="I42" s="5">
         <f>(C42*D42*E42*F42)^(1/4)</f>
         <v>1</v>
       </c>
       <c r="K42" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L42" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="M42"/>
+      <c r="N42" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L42" s="8">
+      <c r="O42" s="7">
         <f>I42/SUM(I$40:I$43)</f>
         <v>0.25</v>
       </c>
-      <c r="M42"/>
-      <c r="N42" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="O42" s="8">
-        <v>0.25</v>
-      </c>
       <c r="Q42" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="R42" s="14">
-        <f>L$40*O49+L$41*P49+L$42*Q49+L$43*R49</f>
-        <v>0.34126162024525425</v>
+      <c r="R42" s="10">
+        <f>O$40*O49+O$41*P49+O$42*Q49+O$43*R49</f>
+        <v>0.25703626406442809</v>
       </c>
       <c r="S42" s="2"/>
       <c r="Y42" s="2"/>
@@ -3568,15 +3565,15 @@
       <c r="B43" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C43" s="6">
+      <c r="C43" s="5">
         <f>1/F40</f>
         <v>1</v>
       </c>
-      <c r="D43" s="6">
+      <c r="D43" s="5">
         <f>1/F41</f>
         <v>1</v>
       </c>
-      <c r="E43" s="6">
+      <c r="E43" s="5">
         <f>1/F42</f>
         <v>1</v>
       </c>
@@ -3587,30 +3584,30 @@
       <c r="H43" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I43" s="6">
+      <c r="I43" s="5">
         <f>(C43*D43*E43*F43)^(1/4)</f>
         <v>1</v>
       </c>
-      <c r="K43" s="3" t="s">
+      <c r="K43" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L43" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="M43"/>
+      <c r="N43" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L43" s="8">
+      <c r="O43" s="7">
         <f>I43/SUM(I$40:I$43)</f>
         <v>0.25</v>
       </c>
-      <c r="M43"/>
-      <c r="N43" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O43" s="8">
-        <v>0.25</v>
-      </c>
       <c r="Q43" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="R43" s="14">
-        <f>L$40*O50+L$41*P50+L$42*Q50+L$43*R50</f>
-        <v>0.32779310164405001</v>
+      <c r="R43" s="10">
+        <f>O$40*O50+O$41*P50+O$42*Q50+O$43*R50</f>
+        <v>0.24686219985231597</v>
       </c>
       <c r="S43" s="2"/>
       <c r="Y43" s="2"/>
@@ -3746,34 +3743,34 @@
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="D47" s="6">
-        <f>(D11^$O$40*J11^$O$41*P11^$O$42*V11^$O$43)^(1/4)</f>
+      <c r="D47" s="5">
+        <f>(D11^$L$40*J11^$L$41*P11^$L$42*V11^$L$43)^(1/4)</f>
         <v>0.96589746929485587</v>
       </c>
-      <c r="E47" s="6">
-        <f>(E11^$O$40*K11^$O$41*Q11^$O$42*W11^$O$43)^(1/4)</f>
+      <c r="E47" s="5">
+        <f>(E11^$L$40*K11^$L$41*Q11^$L$42*W11^$L$43)^(1/4)</f>
         <v>0.97105203132493523</v>
       </c>
-      <c r="F47" s="6">
-        <f>(F11^$O$40*L11^$O$41*R11^$O$42*X11^$O$43)^(1/4)</f>
+      <c r="F47" s="5">
+        <f>(F11^$L$40*L11^$L$41*R11^$L$42*X11^$L$43)^(1/4)</f>
         <v>0.98642490895802559</v>
       </c>
       <c r="H47" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I47" s="6">
+      <c r="I47" s="5">
         <f>(C47*D47*E47)^(1/3)</f>
         <v>0.97886885302890347</v>
       </c>
-      <c r="J47" s="6">
+      <c r="J47" s="5">
         <f>(C54*D54*E54)^(1/3)</f>
         <v>1.055719686630733</v>
       </c>
-      <c r="K47" s="6">
+      <c r="K47" s="5">
         <f>(C61*D61*E61)^(1/3)</f>
         <v>0.95760328069857359</v>
       </c>
-      <c r="L47" s="6">
+      <c r="L47" s="5">
         <f>(C68*D68*E68)^(1/3)</f>
         <v>0.92578758750391754</v>
       </c>
@@ -3781,21 +3778,21 @@
       <c r="N47" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="O47" s="6">
-        <f t="shared" ref="O47:R50" si="0">I47/SUM(I$47:I$49)</f>
-        <v>0.32625176590826066</v>
-      </c>
-      <c r="P47" s="6">
+      <c r="O47" s="5">
+        <f>I47/SUM(I$47:I$50)</f>
+        <v>0.24516537441806305</v>
+      </c>
+      <c r="P47" s="5">
+        <f t="shared" ref="P47:R50" si="0">J47/SUM(J$47:J$50)</f>
+        <v>0.26500907495897857</v>
+      </c>
+      <c r="Q47" s="5">
         <f t="shared" si="0"/>
-        <v>0.35128858570086713</v>
-      </c>
-      <c r="Q47" s="6">
+        <v>0.23928853025548982</v>
+      </c>
+      <c r="R47" s="5">
         <f t="shared" si="0"/>
-        <v>0.31900149824969143</v>
-      </c>
-      <c r="R47" s="6">
-        <f t="shared" si="0"/>
-        <v>0.30809351650841588</v>
+        <v>0.23309797640435237</v>
       </c>
       <c r="S47" s="2"/>
       <c r="Y47" s="2"/>
@@ -3811,7 +3808,7 @@
       <c r="B48" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C48" s="6">
+      <c r="C48" s="5">
         <f>1/D47</f>
         <v>1.0353065742371603</v>
       </c>
@@ -3819,30 +3816,30 @@
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="E48" s="6">
-        <f>(E12^$O$40*K12^$O$41*Q12^$O$42*W12^$O$43)^(1/4)</f>
+      <c r="E48" s="5">
+        <f>(E12^$L$40*K12^$L$41*Q12^$L$42*W12^$L$43)^(1/4)</f>
         <v>1.0053365519570543</v>
       </c>
-      <c r="F48" s="6">
-        <f>(F12^$O$40*L12^$O$41*R12^$O$42*X12^$O$43)^(1/4)</f>
+      <c r="F48" s="5">
+        <f>(F12^$L$40*L12^$L$41*R12^$L$42*X12^$L$43)^(1/4)</f>
         <v>1.0212521932355363</v>
       </c>
       <c r="H48" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I48" s="6">
+      <c r="I48" s="5">
         <f>(C48*D48*E48)^(1/3)</f>
         <v>1.0134293588568124</v>
       </c>
-      <c r="J48" s="6">
+      <c r="J48" s="5">
         <f>(C55*D55*E55)^(1/3)</f>
         <v>0.92025558816108921</v>
       </c>
-      <c r="K48" s="6">
+      <c r="K48" s="5">
         <f>(C62*D62*E62)^(1/3)</f>
         <v>1.0442737824274138</v>
       </c>
-      <c r="L48" s="6">
+      <c r="L48" s="5">
         <f>(C69*D69*E69)^(1/3)</f>
         <v>1.0170378966055869</v>
       </c>
@@ -3850,21 +3847,21 @@
       <c r="N48" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="O48" s="6">
+      <c r="O48" s="5">
+        <f t="shared" ref="O48:O50" si="1">I48/SUM(I$47:I$50)</f>
+        <v>0.25382132391033563</v>
+      </c>
+      <c r="P48" s="5">
         <f t="shared" si="0"/>
-        <v>0.33777059810130533</v>
-      </c>
-      <c r="P48" s="6">
+        <v>0.23100457937155372</v>
+      </c>
+      <c r="Q48" s="5">
         <f t="shared" si="0"/>
-        <v>0.30621318153130461</v>
-      </c>
-      <c r="Q48" s="6">
+        <v>0.26094599258171608</v>
+      </c>
+      <c r="R48" s="5">
         <f t="shared" si="0"/>
-        <v>0.34787360057309119</v>
-      </c>
-      <c r="R48" s="6">
-        <f t="shared" si="0"/>
-        <v>0.33846077244604666</v>
+        <v>0.25607329243253446</v>
       </c>
       <c r="S48" s="2"/>
       <c r="Y48" s="2"/>
@@ -3880,7 +3877,7 @@
       <c r="B49" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C49" s="6">
+      <c r="C49" s="5">
         <f>1/E47</f>
         <v>1.0298109346783069</v>
       </c>
@@ -3892,26 +3889,26 @@
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="F49" s="6">
-        <f>(F13^$O$40*L13^$O$41*R13^$O$42*X13^$O$43)^(1/4)</f>
+      <c r="F49" s="5">
+        <f>(F13^$L$40*L13^$L$41*R13^$L$42*X13^$L$43)^(1/4)</f>
         <v>1.015831157484028</v>
       </c>
       <c r="H49" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I49" s="6">
+      <c r="I49" s="5">
         <f>(C49*D49*E49)^(1/3)</f>
         <v>1.0080498484651772</v>
       </c>
-      <c r="J49" s="6">
+      <c r="J49" s="5">
         <f>(C56*D56*E56)^(1/3)</f>
         <v>1.0293022366434921</v>
       </c>
-      <c r="K49" s="6">
+      <c r="K49" s="5">
         <f>(C63*D63*E63)^(1/3)</f>
         <v>1</v>
       </c>
-      <c r="L49" s="6">
+      <c r="L49" s="5">
         <f>(C70*D70*E70)^(1/3)</f>
         <v>1.0620660111603373</v>
       </c>
@@ -3919,21 +3916,21 @@
       <c r="N49" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O49" s="6">
+      <c r="O49" s="5">
+        <f t="shared" si="1"/>
+        <v>0.25247398338022259</v>
+      </c>
+      <c r="P49" s="5">
         <f t="shared" si="0"/>
-        <v>0.33597763599043406</v>
-      </c>
-      <c r="P49" s="6">
+        <v>0.25837770862892873</v>
+      </c>
+      <c r="Q49" s="5">
         <f t="shared" si="0"/>
-        <v>0.34249823276782831</v>
-      </c>
-      <c r="Q49" s="6">
+        <v>0.24988273858139703</v>
+      </c>
+      <c r="R49" s="5">
         <f t="shared" si="0"/>
-        <v>0.33312490117721733</v>
-      </c>
-      <c r="R49" s="6">
-        <f t="shared" si="0"/>
-        <v>0.3534457110455374</v>
+        <v>0.267410625667164</v>
       </c>
       <c r="S49" s="2"/>
       <c r="Y49" s="2"/>
@@ -3949,15 +3946,15 @@
       <c r="B50" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C50" s="6">
+      <c r="C50" s="5">
         <f>1/F47</f>
         <v>1.0137619102262065</v>
       </c>
-      <c r="D50" s="6">
+      <c r="D50" s="5">
         <f>1/F48</f>
         <v>0.97919006355501181</v>
       </c>
-      <c r="E50" s="6">
+      <c r="E50" s="5">
         <f>1/F49</f>
         <v>0.98441556220500459</v>
       </c>
@@ -3968,19 +3965,19 @@
       <c r="H50" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I50" s="6">
+      <c r="I50" s="5">
         <f>(C50*D50*E50)^(1/3)</f>
         <v>0.99233995830751709</v>
       </c>
-      <c r="J50" s="6">
+      <c r="J50" s="5">
         <f>(C57*D57*E57)^(1/3)</f>
         <v>0.97843393993347616</v>
       </c>
-      <c r="K50" s="6">
+      <c r="K50" s="5">
         <f>(C64*D64*E64)^(1/3)</f>
         <v>1</v>
       </c>
-      <c r="L50" s="6">
+      <c r="L50" s="5">
         <f>(C71*D71*E71)^(1/3)</f>
         <v>0.96677570572706639</v>
       </c>
@@ -3988,21 +3985,21 @@
       <c r="N50" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O50" s="6">
+      <c r="O50" s="5">
+        <f t="shared" si="1"/>
+        <v>0.24853931829137876</v>
+      </c>
+      <c r="P50" s="5">
         <f t="shared" si="0"/>
-        <v>0.3307416134218315</v>
-      </c>
-      <c r="P50" s="6">
+        <v>0.24560863704053904</v>
+      </c>
+      <c r="Q50" s="5">
         <f t="shared" si="0"/>
-        <v>0.3255719101515448</v>
-      </c>
-      <c r="Q50" s="6">
+        <v>0.24988273858139703</v>
+      </c>
+      <c r="R50" s="5">
         <f t="shared" si="0"/>
-        <v>0.33312490117721733</v>
-      </c>
-      <c r="R50" s="6">
-        <f t="shared" si="0"/>
-        <v>0.32173398182560636</v>
+        <v>0.24341810549594914</v>
       </c>
       <c r="S50" s="2"/>
       <c r="Y50" s="2"/>
@@ -4097,16 +4094,16 @@
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="D54" s="6">
-        <f>(D18^$O$40*J18^$O$41*P18^$O$42*V18^$O$43)^(1/4)</f>
+      <c r="D54" s="5">
+        <f>(D18^$L$40*J18^$L$41*P18^$L$42*V18^$L$43)^(1/4)</f>
         <v>1.1472026904398771</v>
       </c>
-      <c r="E54" s="6">
-        <f>(E18^$O$40*K18^$O$41*Q18^$O$42*W18^$O$43)^(1/4)</f>
+      <c r="E54" s="5">
+        <f>(E18^$L$40*K18^$L$41*Q18^$L$42*W18^$L$43)^(1/4)</f>
         <v>1.0256653964664324</v>
       </c>
-      <c r="F54" s="6">
-        <f>(F18^$O$40*L18^$O$41*R18^$O$42*X18^$O$43)^(1/4)</f>
+      <c r="F54" s="5">
+        <f>(F18^$L$40*L18^$L$41*R18^$L$42*X18^$L$43)^(1/4)</f>
         <v>1.0789892332460498</v>
       </c>
       <c r="P54" s="2"/>
@@ -4125,7 +4122,7 @@
       <c r="B55" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C55" s="6">
+      <c r="C55" s="5">
         <f>1/D54</f>
         <v>0.87168554287173572</v>
       </c>
@@ -4133,12 +4130,12 @@
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="E55" s="6">
-        <f>(E19^$O$40*K19^$O$41*Q19^$O$42*W19^$O$43)^(1/4)</f>
+      <c r="E55" s="5">
+        <f>(E19^$L$40*K19^$L$41*Q19^$L$42*W19^$L$43)^(1/4)</f>
         <v>0.89405769792359624</v>
       </c>
-      <c r="F55" s="6">
-        <f>(F19^$O$40*L19^$O$41*R19^$O$42*X19^$O$43)^(1/4)</f>
+      <c r="F55" s="5">
+        <f>(F19^$L$40*L19^$L$41*R19^$L$42*X19^$L$43)^(1/4)</f>
         <v>0.94053931553484071</v>
       </c>
       <c r="P55" s="2"/>
@@ -4157,7 +4154,7 @@
       <c r="B56" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C56" s="6">
+      <c r="C56" s="5">
         <f>1/E54</f>
         <v>0.97497683303458083</v>
       </c>
@@ -4169,8 +4166,8 @@
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="F56" s="6">
-        <f>(F20^$O$40*L20^$O$41*R20^$O$42*X20^$O$43)^(1/4)</f>
+      <c r="F56" s="5">
+        <f>(F20^$L$40*L20^$L$41*R20^$L$42*X20^$L$43)^(1/4)</f>
         <v>1.0519895055086441</v>
       </c>
       <c r="P56" s="2"/>
@@ -4189,15 +4186,15 @@
       <c r="B57" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C57" s="6">
+      <c r="C57" s="5">
         <f>1/F54</f>
         <v>0.92679330728035425</v>
       </c>
-      <c r="D57" s="6">
+      <c r="D57" s="5">
         <f>1/F55</f>
         <v>1.0632197755936941</v>
       </c>
-      <c r="E57" s="6">
+      <c r="E57" s="5">
         <f>1/F56</f>
         <v>0.95057982495414073</v>
       </c>
@@ -4291,16 +4288,16 @@
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="D61" s="6">
-        <f>(D25^$O$40*J25^$O$41*P25^$O$42*V25^$O$43)^(1/4)</f>
+      <c r="D61" s="5">
+        <f>(D25^$L$40*J25^$L$41*P25^$L$42*V25^$L$43)^(1/4)</f>
         <v>0.91700404320467122</v>
       </c>
-      <c r="E61" s="6">
-        <f>(E25^$O$40*K25^$O$41*Q25^$O$42*W25^$O$43)^(1/4)</f>
+      <c r="E61" s="5">
+        <f>(E25^$L$40*K25^$L$41*Q25^$L$42*W25^$L$43)^(1/4)</f>
         <v>0.95760328069857359</v>
       </c>
-      <c r="F61" s="6">
-        <f>(F25^$O$40*L25^$O$41*R25^$O$42*X25^$O$43)^(1/4)</f>
+      <c r="F61" s="5">
+        <f>(F25^$L$40*L25^$L$41*R25^$L$42*X25^$L$43)^(1/4)</f>
         <v>0.95760328069857359</v>
       </c>
       <c r="P61" s="2"/>
@@ -4319,7 +4316,7 @@
       <c r="B62" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C62" s="6">
+      <c r="C62" s="5">
         <f>1/D61</f>
         <v>1.0905077326652577</v>
       </c>
@@ -4327,12 +4324,12 @@
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="E62" s="6">
-        <f>(E26^$O$40*K26^$O$41*Q26^$O$42*W26^$O$43)^(1/4)</f>
+      <c r="E62" s="5">
+        <f>(E26^$L$40*K26^$L$41*Q26^$L$42*W26^$L$43)^(1/4)</f>
         <v>1.0442737824274138</v>
       </c>
-      <c r="F62" s="6">
-        <f>(F26^$O$40*L26^$O$41*R26^$O$42*X26^$O$43)^(1/4)</f>
+      <c r="F62" s="5">
+        <f>(F26^$L$40*L26^$L$41*R26^$L$42*X26^$L$43)^(1/4)</f>
         <v>1.0442737824274138</v>
       </c>
       <c r="P62" s="2"/>
@@ -4351,7 +4348,7 @@
       <c r="B63" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C63" s="6">
+      <c r="C63" s="5">
         <f>1/E61</f>
         <v>1.044273782427414</v>
       </c>
@@ -4363,8 +4360,8 @@
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="F63" s="6">
-        <f>(F27^$O$40*L27^$O$41*R27^$O$42*X27^$O$43)^(1/4)</f>
+      <c r="F63" s="5">
+        <f>(F27^$L$40*L27^$L$41*R27^$L$42*X27^$L$43)^(1/4)</f>
         <v>1</v>
       </c>
       <c r="P63" s="2"/>
@@ -4383,15 +4380,15 @@
       <c r="B64" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C64" s="6">
+      <c r="C64" s="5">
         <f>1/F61</f>
         <v>1.044273782427414</v>
       </c>
-      <c r="D64" s="6">
+      <c r="D64" s="5">
         <f>1/F62</f>
         <v>0.9576032806985737</v>
       </c>
-      <c r="E64" s="6">
+      <c r="E64" s="5">
         <f>1/F63</f>
         <v>1</v>
       </c>
@@ -4512,16 +4509,16 @@
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="D68" s="6">
-        <f>(D32^$O$40*J32^$O$41*P32^$O$42*V32^$O$43)^(1/4)</f>
+      <c r="D68" s="5">
+        <f>(D32^$L$40*J32^$L$41*P32^$L$42*V32^$L$43)^(1/4)</f>
         <v>0.91027835894196096</v>
       </c>
-      <c r="E68" s="6">
-        <f>(E32^$O$40*K32^$O$41*Q32^$O$42*W32^$O$43)^(1/4)</f>
+      <c r="E68" s="5">
+        <f>(E32^$L$40*K32^$L$41*Q32^$L$42*W32^$L$43)^(1/4)</f>
         <v>0.87168554287173572</v>
       </c>
-      <c r="F68" s="6">
-        <f>(F32^$O$40*L32^$O$41*R32^$O$42*X32^$O$43)^(1/4)</f>
+      <c r="F68" s="5">
+        <f>(F32^$L$40*L32^$L$41*R32^$L$42*X32^$L$43)^(1/4)</f>
         <v>0.95760328069857359</v>
       </c>
       <c r="G68" s="2"/>
@@ -4549,7 +4546,7 @@
       <c r="B69" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C69" s="6">
+      <c r="C69" s="5">
         <f>1/D68</f>
         <v>1.0985650599914565</v>
       </c>
@@ -4557,12 +4554,12 @@
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="E69" s="6">
-        <f>(E33^$O$40*K33^$O$41*Q33^$O$42*W33^$O$43)^(1/4)</f>
+      <c r="E69" s="5">
+        <f>(E33^$L$40*K33^$L$41*Q33^$L$42*W33^$L$43)^(1/4)</f>
         <v>0.9576032806985737</v>
       </c>
-      <c r="F69" s="6">
-        <f>(F33^$O$40*L33^$O$41*R33^$O$42*X33^$O$43)^(1/4)</f>
+      <c r="F69" s="5">
+        <f>(F33^$L$40*L33^$L$41*R33^$L$42*X33^$L$43)^(1/4)</f>
         <v>1.0519895055086441</v>
       </c>
       <c r="G69" s="2"/>
@@ -4590,7 +4587,7 @@
       <c r="B70" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C70" s="6">
+      <c r="C70" s="5">
         <f>1/E68</f>
         <v>1.1472026904398771</v>
       </c>
@@ -4602,8 +4599,8 @@
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="F70" s="6">
-        <f>(F34^$O$40*L34^$O$41*R34^$O$42*X34^$O$43)^(1/4)</f>
+      <c r="F70" s="5">
+        <f>(F34^$L$40*L34^$L$41*R34^$L$42*X34^$L$43)^(1/4)</f>
         <v>1.0985650599914565</v>
       </c>
       <c r="G70" s="2"/>
@@ -4631,15 +4628,15 @@
       <c r="B71" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C71" s="6">
+      <c r="C71" s="5">
         <f>1/F68</f>
         <v>1.044273782427414</v>
       </c>
-      <c r="D71" s="6">
+      <c r="D71" s="5">
         <f>1/F69</f>
         <v>0.95057982495414073</v>
       </c>
-      <c r="E71" s="6">
+      <c r="E71" s="5">
         <f>1/F70</f>
         <v>0.91027835894196107</v>
       </c>
@@ -8343,7 +8340,7 @@
   <mergeCells count="31">
     <mergeCell ref="B66:C66"/>
     <mergeCell ref="H38:I38"/>
-    <mergeCell ref="K38:L38"/>
+    <mergeCell ref="N38:O38"/>
     <mergeCell ref="Q38:R38"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="H16:I16"/>
@@ -8353,13 +8350,16 @@
     <mergeCell ref="H23:I23"/>
     <mergeCell ref="N23:O23"/>
     <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="N30:O30"/>
     <mergeCell ref="T16:U16"/>
     <mergeCell ref="T23:U23"/>
     <mergeCell ref="T30:U30"/>
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="T2:U2"/>
     <mergeCell ref="T9:U9"/>
-    <mergeCell ref="N38:O38"/>
+    <mergeCell ref="K38:L38"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="N2:O2"/>
@@ -8369,9 +8369,6 @@
     <mergeCell ref="N9:O9"/>
     <mergeCell ref="H45:I45"/>
     <mergeCell ref="N45:O45"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="N30:O30"/>
   </mergeCells>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>